<commit_message>
feat: Add RC-based AI mode switching system
- Add RC mode controller for RadioMaster integration
- Implement adaptive detector with 'Detect Once, Track Forever'
- Add quantum IMU drift filter for research
- Create installation scripts for Raspberry Pi
- Add comprehensive testing suite
- Update main application with mode switching integration
</commit_message>
<xml_diff>
--- a/FlyingWing_BOM.xlsx
+++ b/FlyingWing_BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NHACNUOC\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\VSCode\Flying_Wing_UAV\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1ECAD7B2-5248-46E5-8C72-ABF2EFA888E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CF8D18C-38E9-4BD2-B456-BAF5B024E55B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{85C5E4E3-B897-4EED-9951-462BCD6A4517}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{85C5E4E3-B897-4EED-9951-462BCD6A4517}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -102,12 +102,6 @@
     <t>Hệ thống động lực</t>
   </si>
   <si>
-    <t>2x DXW D4250 800KV 3-7S Outrunner</t>
-  </si>
-  <si>
-    <t>2 x ESC (Bộ điều tốc) 50A</t>
-  </si>
-  <si>
     <t>IV</t>
   </si>
   <si>
@@ -150,12 +144,6 @@
     <t>801,118 vnđ</t>
   </si>
   <si>
-    <t>Nguồn chính Cấu hình 4S2P - 10400mAh</t>
-  </si>
-  <si>
-    <t>2x Lipo CNHL LVNCell 4s 5200mah 65C</t>
-  </si>
-  <si>
     <t>Tổng chi phí dự tính:</t>
   </si>
   <si>
@@ -192,9 +180,6 @@
     <t>Vật tư phụ (dây điện / keo…)</t>
   </si>
   <si>
-    <t>Thanh carbon</t>
-  </si>
-  <si>
     <t>Camera OV5647 cho Raspberry Pi</t>
   </si>
   <si>
@@ -228,10 +213,25 @@
     <t>FLYING WING UAV - Vật tư phần điện / điều khiển</t>
   </si>
   <si>
-    <t>Nhựa in 3D (Lightweight) - ESUN ePLA-LW</t>
-  </si>
-  <si>
     <t>Nhựa in trọng lượng nhẹ - chuyên UAV (2 cuộn)</t>
+  </si>
+  <si>
+    <t>2x DXW D4250 600KV 3-7S Outrunner</t>
+  </si>
+  <si>
+    <t>2 x ESC (Bộ điều tốc) 100A</t>
+  </si>
+  <si>
+    <t>2x Lipo CNHL LVNCell 6s 5200mah 65C</t>
+  </si>
+  <si>
+    <t>Nguồn chính Cấu hình 6S2P - 10400mAh</t>
+  </si>
+  <si>
+    <t>Thanh carbon phi 16mm</t>
+  </si>
+  <si>
+    <t>Nhựa in 3D</t>
   </si>
 </sst>
 </file>
@@ -240,7 +240,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="170" formatCode="#,##0\ &quot;vnđ&quot;"/>
+    <numFmt numFmtId="164" formatCode="#,##0\ &quot;vnđ&quot;"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -374,9 +374,6 @@
       <alignment horizontal="left" indent="2"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -386,7 +383,35 @@
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
@@ -394,37 +419,12 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="170" fontId="0" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="170" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -742,8 +742,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E60F6C8-D709-4161-92BB-9E713613473A}">
   <dimension ref="A1:D39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K16" sqref="K16"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -755,51 +755,51 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
-        <v>63</v>
-      </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
+      <c r="A1" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="16"/>
-      <c r="B2" s="16" t="s">
+      <c r="A2" s="11"/>
+      <c r="B2" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="C2" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="D2" s="16" t="s">
-        <v>36</v>
-      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="9"/>
-      <c r="D3" s="20"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="14"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="7">
+      <c r="A4" s="6">
         <v>1</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="D4" s="15" t="s">
-        <v>37</v>
+        <v>53</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="7">
+      <c r="A5" s="6">
         <v>2</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -808,12 +808,12 @@
       <c r="C5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="15">
+      <c r="D5" s="10">
         <v>284751</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="7">
+      <c r="A6" s="6">
         <v>3</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -822,44 +822,44 @@
       <c r="C6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="15">
+      <c r="D6" s="10">
         <v>145000</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="7">
+      <c r="A7" s="6">
         <v>7</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="D7" s="15">
+        <v>57</v>
+      </c>
+      <c r="D7" s="10">
         <v>259000</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="7">
+      <c r="A8" s="6">
         <v>4</v>
       </c>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
-      <c r="D8" s="15"/>
+      <c r="D8" s="10"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="8" t="s">
+      <c r="A9" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="10" t="s">
+      <c r="B9" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="11"/>
-      <c r="D9" s="20"/>
+      <c r="C9" s="20"/>
+      <c r="D9" s="14"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="7">
+      <c r="A10" s="6">
         <v>1</v>
       </c>
       <c r="B10" s="2" t="s">
@@ -868,353 +868,353 @@
       <c r="C10" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D10" s="15">
+      <c r="D10" s="10">
         <v>1859000</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="7">
+      <c r="A11" s="6">
         <v>2</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D11" s="15">
+      <c r="D11" s="10">
         <v>469000</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="7"/>
+      <c r="A12" s="6"/>
       <c r="B12" s="3"/>
       <c r="C12" s="1"/>
-      <c r="D12" s="15"/>
+      <c r="D12" s="10"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="12" t="s">
+      <c r="A13" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="9" t="s">
+      <c r="B13" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="9"/>
-      <c r="D13" s="20"/>
+      <c r="C13" s="17"/>
+      <c r="D13" s="14"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="7">
+      <c r="A14" s="6">
         <v>1</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C14" s="5" t="s">
+      <c r="C14" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="D14" s="15" t="s">
-        <v>41</v>
+      <c r="D14" s="10" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="7">
+      <c r="A15" s="6">
         <v>2</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C15" s="5"/>
-      <c r="D15" s="15" t="s">
-        <v>41</v>
+      <c r="C15" s="21"/>
+      <c r="D15" s="10" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="7">
+      <c r="A16" s="6">
         <v>3</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C16" s="5"/>
-      <c r="D16" s="15" t="s">
-        <v>41</v>
+      <c r="C16" s="21"/>
+      <c r="D16" s="10" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="7">
+      <c r="A17" s="6">
         <v>4</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D17" s="15" t="s">
-        <v>41</v>
+      <c r="D17" s="10" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="7">
+      <c r="A18" s="6">
         <v>6</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="D18" s="15">
+        <v>52</v>
+      </c>
+      <c r="D18" s="10">
         <v>50000</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="7"/>
+      <c r="A19" s="6"/>
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
-      <c r="D19" s="15"/>
+      <c r="D19" s="10"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="B20" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="C20" s="13"/>
-      <c r="D20" s="20"/>
+      <c r="A20" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B20" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="C20" s="22"/>
+      <c r="D20" s="14"/>
     </row>
     <row r="21" spans="1:4" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="7">
+      <c r="A21" s="6">
         <v>1</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="D21" s="15" t="s">
-        <v>41</v>
+      <c r="C21" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="D21" s="10" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="7">
+      <c r="A22" s="6">
         <v>2</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C22" s="6"/>
-      <c r="D22" s="15">
+        <v>48</v>
+      </c>
+      <c r="C22" s="5"/>
+      <c r="D22" s="10">
         <v>105000</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="B23" s="9" t="s">
+      <c r="A23" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B23" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="C23" s="9"/>
-      <c r="D23" s="20"/>
+      <c r="C23" s="17"/>
+      <c r="D23" s="14"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="7">
+      <c r="A24" s="6">
         <v>1</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>22</v>
+        <v>60</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D24" s="15">
+        <v>28</v>
+      </c>
+      <c r="D24" s="10">
         <f>510968*2</f>
         <v>1021936</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="7">
+      <c r="A25" s="6">
         <v>2</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>23</v>
+        <v>61</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D25" s="15">
+        <v>27</v>
+      </c>
+      <c r="D25" s="10">
         <f>345000*2</f>
         <v>690000</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="7">
+      <c r="A26" s="6">
         <v>3</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D26" s="15">
+        <v>30</v>
+      </c>
+      <c r="D26" s="10">
         <v>180000</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="7">
+      <c r="A27" s="6">
         <v>4</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="D27" s="15"/>
+        <v>44</v>
+      </c>
+      <c r="D27" s="10"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="B28" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="C28" s="9"/>
-      <c r="D28" s="20"/>
+      <c r="A28" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B28" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="C28" s="17"/>
+      <c r="D28" s="14"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="7">
+      <c r="A29" s="6">
         <v>1</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>39</v>
+        <v>62</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D29" s="15">
+        <v>63</v>
+      </c>
+      <c r="D29" s="10">
         <f>2*780000</f>
         <v>1560000</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="7">
+      <c r="A30" s="6">
         <v>2</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D30" s="15">
+        <v>26</v>
+      </c>
+      <c r="D30" s="10">
         <v>138000</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="7">
+      <c r="A31" s="6">
         <v>3</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D31" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="D31" s="10" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="6">
+        <v>4</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C32" s="1" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="7">
-        <v>4</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C32" s="1" t="s">
+      <c r="D32" s="10">
+        <v>981068</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="9">
+        <v>5</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D33" s="10">
+        <v>15000</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B34" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="D32" s="15">
-        <v>981068</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="14">
-        <v>5</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="C33" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="D33" s="15">
-        <v>15000</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="B34" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="C34" s="9"/>
-      <c r="D34" s="20"/>
+      <c r="C34" s="17"/>
+      <c r="D34" s="14"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="7">
+      <c r="A35" s="6">
         <v>1</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C35" s="1"/>
-      <c r="D35" s="15"/>
+      <c r="D35" s="10"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="7">
+      <c r="A36" s="6">
         <v>2</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>52</v>
+        <v>64</v>
       </c>
       <c r="C36" s="1"/>
-      <c r="D36" s="15"/>
+      <c r="D36" s="10"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="7">
+      <c r="A37" s="6">
         <v>2</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="D37" s="15">
+        <v>59</v>
+      </c>
+      <c r="D37" s="10">
         <f>2*755000</f>
         <v>1510000</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="18">
+      <c r="A38" s="12">
         <v>3</v>
       </c>
-      <c r="B38" s="19"/>
+      <c r="B38" s="13"/>
       <c r="C38" s="1"/>
-      <c r="D38" s="15"/>
+      <c r="D38" s="10"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C39" s="21" t="s">
-        <v>40</v>
-      </c>
-      <c r="D39" s="22">
+      <c r="C39" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="D39" s="16">
         <f>SUM(D3:D38)</f>
         <v>9267755</v>
       </c>

</xml_diff>